<commit_message>
upd. medians and input
</commit_message>
<xml_diff>
--- a/migforecasting/clustering/recommendation system/input.xlsx
+++ b/migforecasting/clustering/recommendation system/input.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>город Боготол</t>
   </si>
@@ -82,6 +82,15 @@
   </si>
   <si>
     <t>clust</t>
+  </si>
+  <si>
+    <t>profile</t>
+  </si>
+  <si>
+    <t>гибрид (лучший)</t>
+  </si>
+  <si>
+    <t>сельхоз (скот)</t>
   </si>
 </sst>
 </file>
@@ -141,7 +150,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -156,6 +165,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -438,18 +450,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="U13" sqref="U13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="21" max="21" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>17</v>
       </c>
@@ -510,8 +523,11 @@
       <c r="T1" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="U1" s="6" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>4706000</v>
       </c>
@@ -571,6 +587,74 @@
       </c>
       <c r="T2" s="2">
         <v>900</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>4706000</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2022</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>5</v>
+      </c>
+      <c r="E3" s="2">
+        <v>-125</v>
+      </c>
+      <c r="F3" s="2">
+        <v>18115</v>
+      </c>
+      <c r="G3" s="2">
+        <v>6034.9999999999991</v>
+      </c>
+      <c r="H3" s="2">
+        <v>26548.188450000001</v>
+      </c>
+      <c r="I3" s="2">
+        <v>14247.099999999989</v>
+      </c>
+      <c r="J3" s="2">
+        <v>414.99999999999989</v>
+      </c>
+      <c r="K3" s="2">
+        <v>701881.48514999985</v>
+      </c>
+      <c r="L3" s="2">
+        <v>29.1</v>
+      </c>
+      <c r="M3" s="2">
+        <v>39.999999999999979</v>
+      </c>
+      <c r="N3" s="2">
+        <v>50.999999999999979</v>
+      </c>
+      <c r="O3" s="2">
+        <v>127.2</v>
+      </c>
+      <c r="P3" s="2">
+        <v>4672.9999999999627</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>11221.57</v>
+      </c>
+      <c r="R3" s="2">
+        <v>56819.699999999822</v>
+      </c>
+      <c r="S3" s="2">
+        <v>5.999999999999992</v>
+      </c>
+      <c r="T3" s="2">
+        <v>900</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Recommsys ver. 0.2 (according to profile)
</commit_message>
<xml_diff>
--- a/migforecasting/clustering/recommendation system/input.xlsx
+++ b/migforecasting/clustering/recommendation system/input.xlsx
@@ -453,12 +453,13 @@
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U13" sqref="U13"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" customWidth="1"/>
     <col min="21" max="21" width="21" customWidth="1"/>
   </cols>
   <sheetData>
@@ -478,53 +479,53 @@
       <c r="E1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="U1" s="6" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -543,53 +544,53 @@
       <c r="E2" s="2">
         <v>-125</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="2">
         <v>18115</v>
       </c>
-      <c r="G2" s="2">
+      <c r="H2" s="2">
         <v>6034.9999999999991</v>
       </c>
-      <c r="H2" s="2">
+      <c r="I2" s="2">
         <v>26548.188450000001</v>
       </c>
-      <c r="I2" s="2">
+      <c r="J2" s="2">
         <v>14247.099999999989</v>
       </c>
-      <c r="J2" s="2">
+      <c r="K2" s="2">
         <v>414.99999999999989</v>
       </c>
-      <c r="K2" s="2">
+      <c r="L2" s="2">
         <v>701881.48514999985</v>
       </c>
-      <c r="L2" s="2">
+      <c r="M2" s="2">
         <v>29.1</v>
       </c>
-      <c r="M2" s="2">
+      <c r="N2" s="2">
         <v>39.999999999999979</v>
       </c>
-      <c r="N2" s="2">
+      <c r="O2" s="2">
         <v>50.999999999999979</v>
       </c>
-      <c r="O2" s="2">
+      <c r="P2" s="2">
         <v>127.2</v>
       </c>
-      <c r="P2" s="2">
+      <c r="Q2" s="2">
         <v>4672.9999999999627</v>
       </c>
-      <c r="Q2" s="2">
+      <c r="R2" s="2">
         <v>11221.57</v>
       </c>
-      <c r="R2" s="2">
+      <c r="S2" s="2">
         <v>56819.699999999822</v>
       </c>
-      <c r="S2" s="2">
+      <c r="T2" s="2">
         <v>5.999999999999992</v>
       </c>
-      <c r="T2" s="2">
+      <c r="U2" s="2">
         <v>900</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
@@ -608,53 +609,53 @@
       <c r="E3" s="2">
         <v>-125</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="2">
         <v>18115</v>
       </c>
-      <c r="G3" s="2">
+      <c r="H3" s="2">
         <v>6034.9999999999991</v>
       </c>
-      <c r="H3" s="2">
+      <c r="I3" s="2">
         <v>26548.188450000001</v>
       </c>
-      <c r="I3" s="2">
+      <c r="J3" s="2">
         <v>14247.099999999989</v>
       </c>
-      <c r="J3" s="2">
+      <c r="K3" s="2">
         <v>414.99999999999989</v>
       </c>
-      <c r="K3" s="2">
+      <c r="L3" s="2">
         <v>701881.48514999985</v>
       </c>
-      <c r="L3" s="2">
+      <c r="M3" s="2">
         <v>29.1</v>
       </c>
-      <c r="M3" s="2">
+      <c r="N3" s="2">
         <v>39.999999999999979</v>
       </c>
-      <c r="N3" s="2">
+      <c r="O3" s="2">
         <v>50.999999999999979</v>
       </c>
-      <c r="O3" s="2">
+      <c r="P3" s="2">
         <v>127.2</v>
       </c>
-      <c r="P3" s="2">
+      <c r="Q3" s="2">
         <v>4672.9999999999627</v>
       </c>
-      <c r="Q3" s="2">
+      <c r="R3" s="2">
         <v>11221.57</v>
       </c>
-      <c r="R3" s="2">
+      <c r="S3" s="2">
         <v>56819.699999999822</v>
       </c>
-      <c r="S3" s="2">
+      <c r="T3" s="2">
         <v>5.999999999999992</v>
       </c>
-      <c r="T3" s="2">
+      <c r="U3" s="2">
         <v>900</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>